<commit_message>
graficas y tablas resumen de cada seroencuta
</commit_message>
<xml_diff>
--- a/SEROFOI/data frame/CRI_HPV16_summary.xlsx
+++ b/SEROFOI/data frame/CRI_HPV16_summary.xlsx
@@ -1,91 +1,98 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caj_d\OneDrive\Escritorio\Proyecto Fuerza de infección VPH\GIT\hpv_seroprevalence\SEROFOI\data frame\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E777BF-6799-4C13-AE6E-2D149D7CA309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t xml:space="preserve">model_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">elpd_loo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">foi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">foi_rhat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">converged</t>
-  </si>
-  <si>
-    <t xml:space="preserve">seroreversion_rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">seroreversion_rate_rhat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">constant_no_seroreversion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-20.6(se=2.9)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.017(95% CI, 0.017-0.018)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">constant_seroreversion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-22.5(se=3.9)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.018(95% CI, 0.017-0.022)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0051(95% CI, 0.00031-0.02)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">time_no_seroreversion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-18.4(se=1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age_no_seroreversion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-18.8(se=0.9)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age_seroreversion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-18.8(se=0.2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1(95% CI, 0.3-1.9)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+  <si>
+    <t>model_name</t>
+  </si>
+  <si>
+    <t>elpd_loo</t>
+  </si>
+  <si>
+    <t>foi</t>
+  </si>
+  <si>
+    <t>foi_rhat</t>
+  </si>
+  <si>
+    <t>converged</t>
+  </si>
+  <si>
+    <t>seroreversion_rate</t>
+  </si>
+  <si>
+    <t>seroreversion_rate_rhat</t>
+  </si>
+  <si>
+    <t>constant_no_seroreversion</t>
+  </si>
+  <si>
+    <t>-20.6(se=2.9)</t>
+  </si>
+  <si>
+    <t>0.017(95% CI, 0.017-0.018)</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>constant_seroreversion</t>
+  </si>
+  <si>
+    <t>-22.5(se=3.9)</t>
+  </si>
+  <si>
+    <t>0.018(95% CI, 0.017-0.022)</t>
+  </si>
+  <si>
+    <t>0.0051(95% CI, 0.00031-0.02)</t>
+  </si>
+  <si>
+    <t>time_no_seroreversion</t>
+  </si>
+  <si>
+    <t>-18.4(se=1)</t>
+  </si>
+  <si>
+    <t>age_no_seroreversion</t>
+  </si>
+  <si>
+    <t>-18.8(se=0.9)</t>
+  </si>
+  <si>
+    <t>age_seroreversion</t>
+  </si>
+  <si>
+    <t>-18.8(se=0.2)</t>
+  </si>
+  <si>
+    <t>1(95% CI, 0.3-1.9)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -121,6 +128,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -402,14 +418,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="A1:G6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="22.88671875" customWidth="1"/>
+    <col min="6" max="6" width="21.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -432,7 +454,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -442,16 +464,14 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F2"/>
-      <c r="G2"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -461,7 +481,7 @@
       <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
@@ -470,61 +490,51 @@
       <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>1</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4"/>
-      <c r="D4"/>
       <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="F4"/>
-      <c r="G4"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="C5"/>
-      <c r="D5"/>
       <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="F5"/>
-      <c r="G5"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="C6"/>
-      <c r="D6"/>
       <c r="E6" t="s">
         <v>10</v>
       </c>
       <c r="F6" t="s">
         <v>21</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>